<commit_message>
add math response and feedback screens
</commit_message>
<xml_diff>
--- a/PyschopyTask/OSPAN/operationSet1_noParen.xlsx
+++ b/PyschopyTask/OSPAN/operationSet1_noParen.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shlab/Documents/GitHub/cgt/PyschopyTask/OSPAN/CGT COG CONT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shlab/Documents/GitHub/cgt/PyschopyTask/OSPAN/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="17060"/>
+    <workbookView xWindow="9240" yWindow="500" windowWidth="28040" windowHeight="17060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,9 +32,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
-    <t>sum</t>
-  </si>
-  <si>
     <t>weight</t>
   </si>
   <si>
@@ -186,6 +183,9 @@
   </si>
   <si>
     <t>8x2</t>
+  </si>
+  <si>
+    <t>problemSum</t>
   </si>
 </sst>
 </file>
@@ -543,7 +543,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -553,16 +553,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -570,7 +570,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -584,7 +584,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -598,7 +598,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -612,7 +612,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -626,7 +626,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -640,7 +640,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>
@@ -654,7 +654,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -668,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -682,7 +682,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1">
         <v>5</v>
@@ -696,7 +696,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -710,7 +710,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1">
         <v>6</v>
@@ -724,7 +724,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1">
         <v>3</v>
@@ -738,7 +738,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
@@ -752,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -766,7 +766,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="1">
         <v>7</v>
@@ -780,7 +780,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
@@ -794,7 +794,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="1">
         <v>8</v>
@@ -808,7 +808,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="1">
         <v>4</v>
@@ -822,7 +822,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
@@ -836,7 +836,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -850,7 +850,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="1">
         <v>9</v>
@@ -864,7 +864,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="1">
         <v>3</v>
@@ -878,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
@@ -892,7 +892,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" s="1">
         <v>2</v>
@@ -906,7 +906,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="1">
         <v>3</v>
@@ -920,7 +920,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" s="1">
         <v>4</v>
@@ -934,7 +934,7 @@
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="1">
         <v>4</v>
@@ -948,7 +948,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" s="1">
         <v>5</v>
@@ -962,7 +962,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="1">
         <v>6</v>
@@ -976,7 +976,7 @@
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" s="1">
         <v>6</v>
@@ -990,7 +990,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" s="1">
         <v>6</v>
@@ -1004,7 +1004,7 @@
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" s="1">
         <v>7</v>
@@ -1018,7 +1018,7 @@
         <v>1</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" s="1">
         <v>8</v>
@@ -1032,7 +1032,7 @@
         <v>1</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" s="1">
         <v>8</v>
@@ -1046,7 +1046,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" s="1">
         <v>8</v>
@@ -1060,7 +1060,7 @@
         <v>1</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37" s="1">
         <v>9</v>
@@ -1074,7 +1074,7 @@
         <v>1</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" s="1">
         <v>9</v>
@@ -1088,7 +1088,7 @@
         <v>1</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39" s="1">
         <v>10</v>
@@ -1102,7 +1102,7 @@
         <v>1</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" s="1">
         <v>10</v>
@@ -1116,7 +1116,7 @@
         <v>1</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C41" s="1">
         <v>12</v>
@@ -1130,7 +1130,7 @@
         <v>1</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C42" s="1">
         <v>12</v>
@@ -1144,7 +1144,7 @@
         <v>1</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C43" s="1">
         <v>12</v>
@@ -1158,7 +1158,7 @@
         <v>1</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44" s="1">
         <v>12</v>
@@ -1172,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45" s="1">
         <v>14</v>
@@ -1186,7 +1186,7 @@
         <v>1</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" s="1">
         <v>14</v>
@@ -1200,7 +1200,7 @@
         <v>1</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C47" s="1">
         <v>15</v>
@@ -1214,7 +1214,7 @@
         <v>1</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C48" s="1">
         <v>15</v>
@@ -1228,7 +1228,7 @@
         <v>1</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C49" s="1">
         <v>16</v>

</xml_diff>